<commit_message>
Arreglos de celdas en solicitudes
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado10/guion03/SolicitudGrafica_CN_10_03_CO.xlsx
+++ b/fuentes/contenidos/grado10/guion03/SolicitudGrafica_CN_10_03_CO.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="hX79YNGfHMUCcosWMoH0GQuhNo2gkebFrfW3do2TOcvwqaujU9m0uwOL5UkRtWEspAy/ISD2JB8+jf057W9mVA==" workbookSaltValue="uRz/CDpmZ5ecKheoN1C0Jw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="20" windowWidth="25680" windowHeight="12660" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14380" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Solicitud gráfica" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="245">
   <si>
     <t>Fecha:</t>
   </si>
@@ -590,37 +590,40 @@
     <t>850 x 400 px</t>
   </si>
   <si>
+    <t>Movimiento en dos dimensiones</t>
+  </si>
+  <si>
+    <t>Sergio Cuellar Ardila</t>
+  </si>
+  <si>
+    <t>Cuaderno de Estudio</t>
+  </si>
+  <si>
     <t>http://upload.wikimedia.org/wikipedia/commons/9/99/Vector_components.png</t>
   </si>
   <si>
-    <t>Movimiento en dos dimensiones</t>
-  </si>
-  <si>
-    <t>Sergio Cuellar Ardila</t>
-  </si>
-  <si>
     <t>Ilustración</t>
   </si>
   <si>
-    <t>Cuaderno de Estudio</t>
+    <t>Suma de vectores</t>
   </si>
   <si>
     <t xml:space="preserve">Distancia de flechas horizonal y vertical deben coincidir con la diagonal </t>
   </si>
   <si>
+    <t>Suma de vetores usando paralelogramo</t>
+  </si>
+  <si>
+    <t>Vector diagonal</t>
+  </si>
+  <si>
     <t>Vector R debe tener una línea más delgada</t>
   </si>
   <si>
     <t>Imagen de autor</t>
   </si>
   <si>
-    <t>Suma de vectores</t>
-  </si>
-  <si>
-    <t>Suma de vetores usando paralelogramo</t>
-  </si>
-  <si>
-    <t>Vector diagonal</t>
+    <t>Fotografía</t>
   </si>
   <si>
     <t>Descomposición de vector diagonal</t>
@@ -647,9 +650,6 @@
     <t>http://upload.wikimedia.org/wikipedia/commons/4/4e/ParabolicWaterTrajectory.jpg</t>
   </si>
   <si>
-    <t>Fotografía</t>
-  </si>
-  <si>
     <t>Fuentes de agua que describen trayectoria parabólica</t>
   </si>
   <si>
@@ -671,12 +671,6 @@
     <t>4 ESO/Física y Química/La cinemática/3 El movimiento rectilíneo uniformemente acelerado/3.2 El movimiento de proyectiles</t>
   </si>
   <si>
-    <t>Descripción del movimiento parabólico</t>
-  </si>
-  <si>
-    <t>La imagen debe modificarse como en la muestra</t>
-  </si>
-  <si>
     <t>Movimiento semiparabólico</t>
   </si>
   <si>
@@ -695,18 +689,18 @@
     <t>Movimiento  circular en una atracción mecánica</t>
   </si>
   <si>
+    <t>Movimiento de satétite</t>
+  </si>
+  <si>
+    <t>Diferentes vectores en distintas posiciones en movimiento circular</t>
+  </si>
+  <si>
     <t>Un satélite artificial en órbita circular alrededor de la tierra, hacer tamaño proporcional, y hacer diferenciación de colores respectivos.</t>
   </si>
   <si>
-    <t>Movimiento de satétite</t>
-  </si>
-  <si>
     <t>Un satélite artificial en órbita circular alrededor de la tierra, hacer tamaño de las flechas IGUAL, y hacer diferenciación de colores respectivos, enumerar subíndices en el mismo orden.</t>
   </si>
   <si>
-    <t>Diferentes vectores en distintas posiciones en movimiento circular</t>
-  </si>
-  <si>
     <t>http://upload.wikimedia.org/wikipedia/commons/1/1a/Circular_motion_velocity_and_acceleration.svg</t>
   </si>
   <si>
@@ -716,13 +710,34 @@
     <t>Se deben realizar todos los vectores rojos de la misma longitud. Al igual que los vectores azules</t>
   </si>
   <si>
+    <t>https://www.flickr.com/photos/95128916@N00/14505761243/in/photolist-o6PPrM-84KBTP-84NJUA-84Leue-xKPE6-cAM1zW-4nFWz3-4ciox6-ekErhw-dp3CR9-d1JFfA-dttGWj-deJQKj-8RNKUN-daKBc7-dkMta1-gPW6Xr-8RKDhX-brdXxC-nc8kz5-cnATwQ-dfAC3C-gPW5Tn-k546xW-2DEdp3-69wHVJ-canLr7-crPJPm-AtPbD-7Ad7Wi-9AeSiN-86GxqW-cUBkKQ-dthKCw-9zRj4d-6VMmmV-8G7dD-46iKM-9QduxJ-81SfW-ciw6Kj-aLRyVD-dmfKpt-dsHTUN-78hQ5U-88ZKgW-9f2h59-iyQgA-bV9EqR-eda8iX</t>
+  </si>
+  <si>
+    <t>http://upload.wikimedia.org/wikipedia/commons/2/22/Nonuniform_circular_motion.svg</t>
+  </si>
+  <si>
+    <t>4° ESO/Física y Química/La gravedad/1 los modelos del universo/1.1 EL modelo de Ptolomeo</t>
+  </si>
+  <si>
+    <t>4° ESO/Física y Química/La gravedad/1 los modelos del universo/1.2 EL modelo de Copérnico</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4° ESO/Física y Química/2 Las leyes de Kepler/2.1 La primera ley de Kepler </t>
+  </si>
+  <si>
+    <t>4° ESO/Física y Química/2 Las leyes de Kepler/2.2 Segunda Ley de Kepler</t>
+  </si>
+  <si>
+    <t>4° ESO/Física y Química/2 Las leyes de Kepler/2.3 Tercera Ley de Kepler</t>
+  </si>
+  <si>
     <t>Componentes vectoriales de  movimiento circular</t>
   </si>
   <si>
     <t xml:space="preserve">El vector azul debe ser paralelo y de igual longitud que la línea punteada. </t>
   </si>
   <si>
-    <t>https://www.flickr.com/photos/95128916@N00/14505761243/in/photolist-o6PPrM-84KBTP-84NJUA-84Leue-xKPE6-cAM1zW-4nFWz3-4ciox6-ekErhw-dp3CR9-d1JFfA-dttGWj-deJQKj-8RNKUN-daKBc7-dkMta1-gPW6Xr-8RKDhX-brdXxC-nc8kz5-cnATwQ-dfAC3C-gPW5Tn-k546xW-2DEdp3-69wHVJ-canLr7-crPJPm-AtPbD-7Ad7Wi-9AeSiN-86GxqW-cUBkKQ-dthKCw-9zRj4d-6VMmmV-8G7dD-46iKM-9QduxJ-81SfW-ciw6Kj-aLRyVD-dmfKpt-dsHTUN-78hQ5U-88ZKgW-9f2h59-iyQgA-bV9EqR-eda8iX</t>
+    <t>Movimiento circular uniformemente acelerado</t>
   </si>
   <si>
     <t>La imagen debe ser creada. 
@@ -730,49 +745,25 @@
 En la figura poner coma en los decimales: 1,0 y 2,0</t>
   </si>
   <si>
-    <t>Movimiento circular uniformemente acelerado</t>
-  </si>
-  <si>
-    <t>http://upload.wikimedia.org/wikipedia/commons/2/22/Nonuniform_circular_motion.svg</t>
-  </si>
-  <si>
     <t>Componentes aceleración movimiento circular acelerado</t>
   </si>
   <si>
     <t>Prestar atención a la flecha circular y a los vectores deben ser más notables en grosor que la circunferencia</t>
   </si>
   <si>
-    <t>4° ESO/Física y Química/La gravedad/1 los modelos del universo/1.1 EL modelo de Ptolomeo</t>
-  </si>
-  <si>
     <t>Modelo de Ptolomeo</t>
   </si>
   <si>
-    <t>4° ESO/Física y Química/La gravedad/1 los modelos del universo/1.2 EL modelo de Copérnico</t>
-  </si>
-  <si>
     <t>Modelo de Copérnico</t>
   </si>
   <si>
-    <t xml:space="preserve">4° ESO/Física y Química/2 Las leyes de Kepler/2.1 La primera ley de Kepler </t>
-  </si>
-  <si>
     <t>Primera ley de Kepler</t>
   </si>
   <si>
-    <t>4° ESO/Física y Química/2 Las leyes de Kepler/2.2 Segunda Ley de Kepler</t>
-  </si>
-  <si>
     <t>Segunda ley de Kepler</t>
   </si>
   <si>
-    <t>4° ESO/Física y Química/2 Las leyes de Kepler/2.3 Tercera Ley de Kepler</t>
-  </si>
-  <si>
     <t>Tercera ley de Kepler</t>
-  </si>
-  <si>
-    <t>CN_10_03_CO</t>
   </si>
 </sst>
 </file>
@@ -782,7 +773,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -929,16 +920,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF333333"/>
-      <name val="Arial"/>
-    </font>
   </fonts>
   <fills count="9">
     <fill>
@@ -988,7 +969,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="37">
+  <borders count="36">
     <border>
       <left/>
       <right/>
@@ -1433,23 +1414,8 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="55">
+  <cellStyleXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1503,10 +1469,8 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="112">
+  <cellXfs count="106">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1817,20 +1781,8 @@
     <xf numFmtId="0" fontId="15" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="51"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="36" xfId="51" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="51" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="55">
+  <cellStyles count="53">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="5" builtinId="8" hidden="1"/>
@@ -1856,7 +1808,7 @@
     <cellStyle name="Hipervínculo" xfId="45" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="47" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="49" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="51" builtinId="8"/>
+    <cellStyle name="Hipervínculo" xfId="51" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="6" builtinId="9" hidden="1"/>
@@ -1883,8 +1835,6 @@
     <cellStyle name="Hipervínculo visitado" xfId="48" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="50" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="52" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="53" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="54" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="1">
@@ -1927,15 +1877,15 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropStyle="combo" dx="33" fmlaLink="$H$20" fmlaRange="$H$4:$H$7" noThreeD="1" sel="2" val="0"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropStyle="combo" dx="33" fmlaLink="$H$20" fmlaRange="$H$4:$H$7" noThreeD="1" sel="4" val="0"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="9" dropStyle="combo" dx="33" fmlaLink="$I$20" fmlaRange="$I$6:$I$14" noThreeD="1" sel="8" val="0"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="9" dropStyle="combo" dx="33" fmlaLink="$I$20" fmlaRange="$I$6:$I$14" noThreeD="1" sel="5" val="0"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp3.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="16" dropStyle="combo" dx="33" fmlaLink="$J$20" fmlaRange="$J$4:$J$19" noThreeD="1" sel="3" val="0"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="16" dropStyle="combo" dx="33" fmlaLink="$J$20" fmlaRange="$J$4:$J$19" noThreeD="1" sel="4" val="0"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp4.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1943,15 +1893,15 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp5.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="54" dropStyle="combo" dx="33" fmlaLink="$H$20" fmlaRange="$H$4:$H$7" noThreeD="1" sel="2" val="0"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropStyle="combo" dx="33" fmlaLink="$H$20" fmlaRange="$H$4:$H$7" noThreeD="1" sel="4" val="0"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp6.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="54" dropStyle="combo" dx="33" fmlaLink="$I$20" fmlaRange="$I$6:$I$14" noThreeD="1" sel="8" val="0"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="9" dropStyle="combo" dx="33" fmlaLink="$I$20" fmlaRange="$I$6:$I$14" noThreeD="1" sel="5" val="0"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp7.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="54" dropStyle="combo" dx="33" fmlaLink="$J$20" fmlaRange="$J$4:$J$19" noThreeD="1" sel="3" val="0"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="16" dropStyle="combo" dx="33" fmlaLink="$J$20" fmlaRange="$J$4:$J$19" noThreeD="1" sel="4" val="0"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2007,8 +1957,8 @@
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>4</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>863600</xdr:colOff>
           <xdr:row>4</xdr:row>
           <xdr:rowOff>228600</xdr:rowOff>
         </xdr:to>
@@ -2171,8 +2121,8 @@
           <xdr:rowOff>482600</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>838200</xdr:colOff>
           <xdr:row>15</xdr:row>
           <xdr:rowOff>711200</xdr:rowOff>
         </xdr:to>
@@ -2212,8 +2162,8 @@
           <xdr:rowOff>482600</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>6</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>838200</xdr:colOff>
           <xdr:row>15</xdr:row>
           <xdr:rowOff>711200</xdr:rowOff>
         </xdr:to>
@@ -2571,15 +2521,15 @@
   <sheetPr codeName="Hoja1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:P108"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B35" sqref="B35"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <pane ySplit="9" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="7" style="2" customWidth="1"/>
-    <col min="2" max="2" width="31.1640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="21" style="2" customWidth="1"/>
     <col min="3" max="3" width="21.1640625" style="2" customWidth="1"/>
     <col min="4" max="4" width="15.5" style="2" customWidth="1"/>
     <col min="5" max="5" width="17.1640625" style="2" customWidth="1"/>
@@ -2588,7 +2538,7 @@
     <col min="8" max="8" width="28.6640625" style="2" customWidth="1"/>
     <col min="9" max="9" width="20.5" style="2" customWidth="1"/>
     <col min="10" max="10" width="34.83203125" style="16" customWidth="1"/>
-    <col min="11" max="11" width="121.5" style="16" customWidth="1"/>
+    <col min="11" max="11" width="60.33203125" style="16" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="20.33203125" style="2" hidden="1" customWidth="1"/>
     <col min="13" max="13" width="14.5" style="2" hidden="1" customWidth="1"/>
     <col min="14" max="15" width="0" style="2" hidden="1" customWidth="1"/>
@@ -2674,7 +2624,7 @@
         <v>54</v>
       </c>
       <c r="C4" s="84" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D4" s="85"/>
       <c r="E4" s="5"/>
@@ -2682,7 +2632,7 @@
         <v>55</v>
       </c>
       <c r="G4" s="62" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="H4" s="59"/>
       <c r="I4" s="39"/>
@@ -2702,7 +2652,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="86" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D5" s="87"/>
       <c r="E5" s="5"/>
@@ -2828,20 +2778,20 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:16" s="12" customFormat="1" ht="15">
+    <row r="10" spans="1:16" s="12" customFormat="1" ht="52">
       <c r="A10" s="13" t="str">
         <f>IF(OR(B10&lt;&gt;"",J10&lt;&gt;""),"IMG01","")</f>
         <v>IMG01</v>
       </c>
-      <c r="B10" s="107" t="s">
-        <v>187</v>
+      <c r="B10" s="63" t="s">
+        <v>190</v>
       </c>
       <c r="C10" s="21" t="str">
         <f t="shared" ref="C10:C41" si="0">IF(OR(B10&lt;&gt;"",J10&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D10" s="64" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="E10" s="64" t="s">
         <v>156</v>
@@ -2863,26 +2813,26 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J10" s="64" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="K10" s="65" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" s="12" customFormat="1" ht="15">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" s="12" customFormat="1" ht="53" customHeight="1">
       <c r="A11" s="13" t="str">
         <f t="shared" ref="A11:A18" si="3">IF(OR(B11&lt;&gt;"",J11&lt;&gt;""),CONCATENATE(LEFT(A10,3),IF(MID(A10,4,2)+1&lt;10,CONCATENATE("0",MID(A10,4,2)+1))),"")</f>
         <v>IMG02</v>
       </c>
-      <c r="B11" s="107" t="s">
-        <v>187</v>
+      <c r="B11" s="63" t="s">
+        <v>190</v>
       </c>
       <c r="C11" s="21" t="str">
         <f t="shared" si="0"/>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D11" s="64" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="E11" s="64" t="s">
         <v>156</v>
@@ -2904,28 +2854,30 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J11" s="65" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="K11" s="65" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" s="12" customFormat="1" ht="15">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" s="12" customFormat="1" ht="52">
       <c r="A12" s="13" t="str">
         <f t="shared" si="3"/>
         <v>IMG03</v>
       </c>
-      <c r="B12" s="107" t="s">
-        <v>187</v>
+      <c r="B12" s="63" t="s">
+        <v>190</v>
       </c>
       <c r="C12" s="21" t="str">
         <f t="shared" si="0"/>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D12" s="64" t="s">
-        <v>190</v>
-      </c>
-      <c r="E12" s="64"/>
+        <v>191</v>
+      </c>
+      <c r="E12" s="64" t="s">
+        <v>156</v>
+      </c>
       <c r="F12" s="14" t="str">
         <f t="shared" si="4"/>
         <v>CN_08_01_REC10_IMG03_small</v>
@@ -2943,10 +2895,10 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J12" s="65" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="K12" s="65" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
     </row>
     <row r="13" spans="1:16" s="12" customFormat="1">
@@ -2955,14 +2907,14 @@
         <v>IMG04</v>
       </c>
       <c r="B13" s="63" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="C13" s="21" t="str">
         <f t="shared" si="0"/>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D13" s="64" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="E13" s="64" t="s">
         <v>156</v>
@@ -2984,10 +2936,10 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J13" s="65" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="K13" s="65" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row r="14" spans="1:16" s="12" customFormat="1">
@@ -2996,14 +2948,14 @@
         <v>IMG05</v>
       </c>
       <c r="B14" s="63" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="C14" s="21" t="str">
         <f t="shared" si="0"/>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D14" s="64" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="E14" s="64" t="s">
         <v>157</v>
@@ -3025,10 +2977,10 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J14" s="65" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="K14" s="65" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="15" spans="1:16" s="12" customFormat="1">
@@ -3037,14 +2989,14 @@
         <v>IMG06</v>
       </c>
       <c r="B15" s="63" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="C15" s="21" t="str">
         <f t="shared" si="0"/>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D15" s="64" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="E15" s="64" t="s">
         <v>156</v>
@@ -3066,26 +3018,26 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J15" s="67" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="K15" s="67" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" s="12" customFormat="1" ht="27" thickBot="1">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" s="12" customFormat="1" ht="26">
       <c r="A16" s="13" t="str">
         <f t="shared" si="3"/>
         <v>IMG07</v>
       </c>
       <c r="B16" s="63" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="C16" s="21" t="str">
         <f t="shared" si="0"/>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D16" s="64" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="E16" s="64" t="s">
         <v>156</v>
@@ -3107,26 +3059,26 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J16" s="67" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="K16" s="69" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" s="12" customFormat="1" ht="46" thickBot="1">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" s="12" customFormat="1" ht="52">
       <c r="A17" s="13" t="str">
         <f t="shared" si="3"/>
         <v>IMG08</v>
       </c>
-      <c r="B17" s="108" t="s">
-        <v>205</v>
+      <c r="B17" s="63" t="s">
+        <v>206</v>
       </c>
       <c r="C17" s="21" t="str">
         <f t="shared" si="0"/>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D17" s="64" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="E17" s="64" t="s">
         <v>156</v>
@@ -3152,12 +3104,12 @@
       </c>
       <c r="K17" s="67"/>
     </row>
-    <row r="18" spans="1:11" s="12" customFormat="1" ht="26">
+    <row r="18" spans="1:11" s="12" customFormat="1" ht="52">
       <c r="A18" s="13" t="str">
         <f t="shared" si="3"/>
         <v>IMG09</v>
       </c>
-      <c r="B18" s="109" t="s">
+      <c r="B18" s="63" t="s">
         <v>208</v>
       </c>
       <c r="C18" s="21" t="str">
@@ -3165,7 +3117,7 @@
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D18" s="64" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="E18" s="64" t="s">
         <v>156</v>
@@ -3191,12 +3143,12 @@
       </c>
       <c r="K18" s="67"/>
     </row>
-    <row r="19" spans="1:11" s="12" customFormat="1" ht="26">
+    <row r="19" spans="1:11" s="12" customFormat="1" ht="52">
       <c r="A19" s="13" t="str">
         <f t="shared" ref="A19:A50" si="6">IF(OR(B19&lt;&gt;"",J19&lt;&gt;""),CONCATENATE(LEFT(A18,3),IF(MID(A18,4,2)+1&lt;10,CONCATENATE("0",MID(A18,4,2)+1),MID(A18,4,2)+1)),"")</f>
         <v>IMG10</v>
       </c>
-      <c r="B19" s="109" t="s">
+      <c r="B19" s="63" t="s">
         <v>210</v>
       </c>
       <c r="C19" s="21" t="str">
@@ -3204,7 +3156,7 @@
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D19" s="64" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="E19" s="64" t="s">
         <v>156</v>
@@ -3232,12 +3184,12 @@
         <v>212</v>
       </c>
     </row>
-    <row r="20" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="20" spans="1:11" s="12" customFormat="1" ht="104">
       <c r="A20" s="13" t="str">
         <f t="shared" si="6"/>
         <v>IMG11</v>
       </c>
-      <c r="B20" s="106" t="s">
+      <c r="B20" s="63" t="s">
         <v>213</v>
       </c>
       <c r="C20" s="21" t="str">
@@ -3245,7 +3197,7 @@
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D20" s="64" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="E20" s="64" t="s">
         <v>156</v>
@@ -3266,19 +3218,19 @@
         <f ca="1">IF(OR($B20&lt;&gt;"",$J20&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E20,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E20,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J20" s="65" t="s">
+      <c r="J20" s="67" t="s">
         <v>214</v>
       </c>
       <c r="K20" s="67" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="21" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="21" spans="1:11" s="12" customFormat="1" ht="52">
       <c r="A21" s="13" t="str">
         <f t="shared" si="6"/>
         <v>IMG12</v>
       </c>
-      <c r="B21" s="109" t="s">
+      <c r="B21" s="63" t="s">
         <v>210</v>
       </c>
       <c r="C21" s="21" t="str">
@@ -3286,7 +3238,7 @@
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D21" s="64" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="E21" s="64" t="s">
         <v>156</v>
@@ -3307,27 +3259,23 @@
         <f ca="1">IF(OR($B21&lt;&gt;"",$J21&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E21,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E21,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J21" s="67" t="s">
-        <v>216</v>
-      </c>
-      <c r="K21" s="67" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" s="12" customFormat="1" ht="26">
+      <c r="J21" s="67"/>
+      <c r="K21" s="67"/>
+    </row>
+    <row r="22" spans="1:11" s="12" customFormat="1" ht="273">
       <c r="A22" s="13" t="str">
         <f t="shared" si="6"/>
         <v>IMG13</v>
       </c>
-      <c r="B22" s="109" t="s">
-        <v>218</v>
+      <c r="B22" s="63" t="s">
+        <v>216</v>
       </c>
       <c r="C22" s="21" t="str">
         <f t="shared" si="0"/>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D22" s="64" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="E22" s="64" t="s">
         <v>156</v>
@@ -3349,24 +3297,24 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J22" s="64" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="K22" s="70"/>
     </row>
-    <row r="23" spans="1:11" s="12" customFormat="1" ht="195">
+    <row r="23" spans="1:11" s="12" customFormat="1" ht="273">
       <c r="A23" s="13" t="str">
         <f t="shared" si="6"/>
         <v>IMG14</v>
       </c>
       <c r="B23" s="63" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C23" s="21" t="str">
         <f t="shared" si="0"/>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D23" s="64" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="E23" s="64" t="s">
         <v>156</v>
@@ -3388,24 +3336,24 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J23" s="65" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="K23" s="65"/>
     </row>
-    <row r="24" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="24" spans="1:11" s="12" customFormat="1" ht="26">
       <c r="A24" s="13" t="str">
         <f t="shared" si="6"/>
         <v>IMG15</v>
       </c>
       <c r="B24" s="63" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="C24" s="21" t="str">
         <f t="shared" si="0"/>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D24" s="64" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="E24" s="64" t="s">
         <v>157</v>
@@ -3427,26 +3375,26 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J24" s="64" t="s">
-        <v>223</v>
-      </c>
-      <c r="K24" s="110" t="s">
+        <v>220</v>
+      </c>
+      <c r="K24" s="66" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="25" spans="1:11" s="12" customFormat="1" ht="30">
+    <row r="25" spans="1:11" s="12" customFormat="1" ht="39">
       <c r="A25" s="13" t="str">
         <f t="shared" si="6"/>
         <v>IMG16</v>
       </c>
       <c r="B25" s="63" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="C25" s="21" t="str">
         <f t="shared" si="0"/>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D25" s="64" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="E25" s="64" t="s">
         <v>157</v>
@@ -3468,29 +3416,29 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J25" s="64" t="s">
-        <v>225</v>
-      </c>
-      <c r="K25" s="111" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" s="12" customFormat="1" ht="15">
+        <v>221</v>
+      </c>
+      <c r="K25" s="65" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" s="12" customFormat="1" ht="65">
       <c r="A26" s="13" t="str">
         <f t="shared" si="6"/>
         <v>IMG17</v>
       </c>
-      <c r="B26" s="107" t="s">
-        <v>226</v>
+      <c r="B26" s="63" t="s">
+        <v>224</v>
       </c>
       <c r="C26" s="21" t="str">
         <f t="shared" si="0"/>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D26" s="64" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="E26" s="64" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="F26" s="14" t="str">
         <f t="shared" si="4"/>
@@ -3509,10 +3457,10 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J26" s="64" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="K26" s="65" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="27" spans="1:11" s="12" customFormat="1" ht="26">
@@ -3521,14 +3469,14 @@
         <v>IMG18</v>
       </c>
       <c r="B27" s="63" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="C27" s="21" t="str">
         <f t="shared" si="0"/>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D27" s="64" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="E27" s="64" t="s">
         <v>156</v>
@@ -3550,26 +3498,26 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J27" s="65" t="s">
-        <v>229</v>
+        <v>234</v>
       </c>
       <c r="K27" s="65" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" s="12" customFormat="1" ht="195">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" s="12" customFormat="1" ht="273">
       <c r="A28" s="13" t="str">
         <f t="shared" si="6"/>
         <v>IMG19</v>
       </c>
       <c r="B28" s="63" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="C28" s="21" t="str">
         <f t="shared" si="0"/>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D28" s="64" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="E28" s="64" t="s">
         <v>156</v>
@@ -3591,26 +3539,26 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J28" s="65" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="K28" s="65" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" s="12" customFormat="1" ht="39">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" s="12" customFormat="1" ht="52">
       <c r="A29" s="13" t="str">
         <f t="shared" si="6"/>
         <v>IMG20</v>
       </c>
       <c r="B29" s="63" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="C29" s="21" t="str">
         <f t="shared" si="0"/>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D29" s="64" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="E29" s="64" t="s">
         <v>156</v>
@@ -3632,26 +3580,26 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J29" s="65" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="K29" s="65" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" s="12" customFormat="1" ht="39">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" s="12" customFormat="1" ht="78">
       <c r="A30" s="13" t="str">
         <f t="shared" si="6"/>
         <v>IMG21</v>
       </c>
       <c r="B30" s="63" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
       <c r="C30" s="21" t="str">
         <f t="shared" si="0"/>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D30" s="64" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="E30" s="64" t="s">
         <v>156</v>
@@ -3673,24 +3621,24 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J30" s="65" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="K30" s="65"/>
     </row>
-    <row r="31" spans="1:11" s="12" customFormat="1" ht="52">
+    <row r="31" spans="1:11" s="12" customFormat="1" ht="78">
       <c r="A31" s="13" t="str">
         <f t="shared" si="6"/>
         <v>IMG22</v>
       </c>
       <c r="B31" s="63" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
       <c r="C31" s="21" t="str">
         <f t="shared" si="0"/>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D31" s="64" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="E31" s="64" t="s">
         <v>156</v>
@@ -3712,24 +3660,24 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J31" s="65" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="K31" s="65"/>
     </row>
-    <row r="32" spans="1:11" s="12" customFormat="1" ht="39">
+    <row r="32" spans="1:11" s="12" customFormat="1" ht="52">
       <c r="A32" s="13" t="str">
         <f t="shared" si="6"/>
         <v>IMG23</v>
       </c>
       <c r="B32" s="63" t="s">
-        <v>241</v>
+        <v>231</v>
       </c>
       <c r="C32" s="21" t="str">
         <f t="shared" si="0"/>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D32" s="64" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="E32" s="64" t="s">
         <v>156</v>
@@ -3755,20 +3703,20 @@
       </c>
       <c r="K32" s="65"/>
     </row>
-    <row r="33" spans="1:11" s="12" customFormat="1" ht="39">
+    <row r="33" spans="1:11" s="12" customFormat="1" ht="52">
       <c r="A33" s="13" t="str">
         <f t="shared" si="6"/>
         <v>IMG24</v>
       </c>
       <c r="B33" s="63" t="s">
-        <v>243</v>
+        <v>232</v>
       </c>
       <c r="C33" s="21" t="str">
         <f t="shared" si="0"/>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D33" s="64" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="E33" s="64" t="s">
         <v>156</v>
@@ -3790,24 +3738,24 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J33" s="65" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="K33" s="65"/>
     </row>
-    <row r="34" spans="1:11" s="12" customFormat="1" ht="26">
+    <row r="34" spans="1:11" s="12" customFormat="1" ht="52">
       <c r="A34" s="13" t="str">
         <f t="shared" si="6"/>
         <v>IMG25</v>
       </c>
       <c r="B34" s="63" t="s">
-        <v>245</v>
+        <v>233</v>
       </c>
       <c r="C34" s="21" t="str">
         <f t="shared" si="0"/>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D34" s="64" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="E34" s="64" t="s">
         <v>156</v>
@@ -3829,11 +3777,11 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J34" s="65" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="K34" s="65"/>
     </row>
-    <row r="35" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="35" spans="1:11" s="12" customFormat="1">
       <c r="A35" s="13" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3864,7 +3812,7 @@
       <c r="J35" s="64"/>
       <c r="K35" s="66"/>
     </row>
-    <row r="36" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="36" spans="1:11" s="12" customFormat="1">
       <c r="A36" s="13" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3895,7 +3843,7 @@
       <c r="J36" s="64"/>
       <c r="K36" s="66"/>
     </row>
-    <row r="37" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="37" spans="1:11" s="12" customFormat="1">
       <c r="A37" s="13" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3926,7 +3874,7 @@
       <c r="J37" s="71"/>
       <c r="K37" s="66"/>
     </row>
-    <row r="38" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="38" spans="1:11" s="12" customFormat="1">
       <c r="A38" s="13" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3957,7 +3905,7 @@
       <c r="J38" s="72"/>
       <c r="K38" s="66"/>
     </row>
-    <row r="39" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="39" spans="1:11" s="12" customFormat="1">
       <c r="A39" s="13" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3988,7 +3936,7 @@
       <c r="J39" s="64"/>
       <c r="K39" s="66"/>
     </row>
-    <row r="40" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="40" spans="1:11" s="12" customFormat="1">
       <c r="A40" s="13" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -4019,7 +3967,7 @@
       <c r="J40" s="64"/>
       <c r="K40" s="66"/>
     </row>
-    <row r="41" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="41" spans="1:11" s="12" customFormat="1">
       <c r="A41" s="13" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -4050,7 +3998,7 @@
       <c r="J41" s="64"/>
       <c r="K41" s="66"/>
     </row>
-    <row r="42" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="42" spans="1:11" s="12" customFormat="1">
       <c r="A42" s="13" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -4081,7 +4029,7 @@
       <c r="J42" s="64"/>
       <c r="K42" s="66"/>
     </row>
-    <row r="43" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="43" spans="1:11" s="12" customFormat="1">
       <c r="A43" s="13" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -4112,7 +4060,7 @@
       <c r="J43" s="64"/>
       <c r="K43" s="66"/>
     </row>
-    <row r="44" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="44" spans="1:11" s="12" customFormat="1">
       <c r="A44" s="13" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -4143,7 +4091,7 @@
       <c r="J44" s="64"/>
       <c r="K44" s="66"/>
     </row>
-    <row r="45" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="45" spans="1:11" s="12" customFormat="1">
       <c r="A45" s="13" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -4174,7 +4122,7 @@
       <c r="J45" s="64"/>
       <c r="K45" s="66"/>
     </row>
-    <row r="46" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="46" spans="1:11" s="12" customFormat="1">
       <c r="A46" s="13" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -4205,7 +4153,7 @@
       <c r="J46" s="64"/>
       <c r="K46" s="66"/>
     </row>
-    <row r="47" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="47" spans="1:11" s="12" customFormat="1">
       <c r="A47" s="13" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -4236,7 +4184,7 @@
       <c r="J47" s="64"/>
       <c r="K47" s="66"/>
     </row>
-    <row r="48" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="48" spans="1:11" s="12" customFormat="1">
       <c r="A48" s="13" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -4267,7 +4215,7 @@
       <c r="J48" s="64"/>
       <c r="K48" s="66"/>
     </row>
-    <row r="49" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="49" spans="1:11" s="12" customFormat="1">
       <c r="A49" s="13" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -4298,7 +4246,7 @@
       <c r="J49" s="64"/>
       <c r="K49" s="66"/>
     </row>
-    <row r="50" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="50" spans="1:11" s="12" customFormat="1">
       <c r="A50" s="13" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -4329,7 +4277,7 @@
       <c r="J50" s="64"/>
       <c r="K50" s="66"/>
     </row>
-    <row r="51" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="51" spans="1:11" s="12" customFormat="1">
       <c r="A51" s="13" t="str">
         <f t="shared" ref="A51:A82" si="8">IF(OR(B51&lt;&gt;"",J51&lt;&gt;""),CONCATENATE(LEFT(A50,3),IF(MID(A50,4,2)+1&lt;10,CONCATENATE("0",MID(A50,4,2)+1),MID(A50,4,2)+1)),"")</f>
         <v/>
@@ -4360,7 +4308,7 @@
       <c r="J51" s="64"/>
       <c r="K51" s="66"/>
     </row>
-    <row r="52" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="52" spans="1:11" s="12" customFormat="1">
       <c r="A52" s="13" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4391,7 +4339,7 @@
       <c r="J52" s="64"/>
       <c r="K52" s="66"/>
     </row>
-    <row r="53" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="53" spans="1:11" s="12" customFormat="1">
       <c r="A53" s="13" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4422,7 +4370,7 @@
       <c r="J53" s="64"/>
       <c r="K53" s="66"/>
     </row>
-    <row r="54" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="54" spans="1:11" s="12" customFormat="1">
       <c r="A54" s="13" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4453,7 +4401,7 @@
       <c r="J54" s="64"/>
       <c r="K54" s="66"/>
     </row>
-    <row r="55" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="55" spans="1:11" s="12" customFormat="1">
       <c r="A55" s="13" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4484,7 +4432,7 @@
       <c r="J55" s="64"/>
       <c r="K55" s="66"/>
     </row>
-    <row r="56" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="56" spans="1:11" s="12" customFormat="1">
       <c r="A56" s="13" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4515,7 +4463,7 @@
       <c r="J56" s="64"/>
       <c r="K56" s="66"/>
     </row>
-    <row r="57" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="57" spans="1:11" s="12" customFormat="1">
       <c r="A57" s="13" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4546,7 +4494,7 @@
       <c r="J57" s="64"/>
       <c r="K57" s="66"/>
     </row>
-    <row r="58" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="58" spans="1:11" s="12" customFormat="1">
       <c r="A58" s="13" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4577,7 +4525,7 @@
       <c r="J58" s="64"/>
       <c r="K58" s="66"/>
     </row>
-    <row r="59" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="59" spans="1:11" s="12" customFormat="1">
       <c r="A59" s="13" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4608,7 +4556,7 @@
       <c r="J59" s="64"/>
       <c r="K59" s="66"/>
     </row>
-    <row r="60" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="60" spans="1:11" s="12" customFormat="1">
       <c r="A60" s="13" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4639,7 +4587,7 @@
       <c r="J60" s="64"/>
       <c r="K60" s="66"/>
     </row>
-    <row r="61" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="61" spans="1:11" s="12" customFormat="1">
       <c r="A61" s="13" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4670,7 +4618,7 @@
       <c r="J61" s="64"/>
       <c r="K61" s="66"/>
     </row>
-    <row r="62" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="62" spans="1:11" s="12" customFormat="1">
       <c r="A62" s="13" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4701,7 +4649,7 @@
       <c r="J62" s="64"/>
       <c r="K62" s="66"/>
     </row>
-    <row r="63" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="63" spans="1:11" s="12" customFormat="1">
       <c r="A63" s="13" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4732,7 +4680,7 @@
       <c r="J63" s="64"/>
       <c r="K63" s="66"/>
     </row>
-    <row r="64" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="64" spans="1:11" s="12" customFormat="1">
       <c r="A64" s="13" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4763,7 +4711,7 @@
       <c r="J64" s="64"/>
       <c r="K64" s="66"/>
     </row>
-    <row r="65" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="65" spans="1:11" s="12" customFormat="1">
       <c r="A65" s="13" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4794,7 +4742,7 @@
       <c r="J65" s="64"/>
       <c r="K65" s="66"/>
     </row>
-    <row r="66" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="66" spans="1:11" s="12" customFormat="1">
       <c r="A66" s="13" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4825,7 +4773,7 @@
       <c r="J66" s="64"/>
       <c r="K66" s="66"/>
     </row>
-    <row r="67" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="67" spans="1:11" s="12" customFormat="1">
       <c r="A67" s="13" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4856,7 +4804,7 @@
       <c r="J67" s="64"/>
       <c r="K67" s="66"/>
     </row>
-    <row r="68" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="68" spans="1:11" s="12" customFormat="1">
       <c r="A68" s="13" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4887,7 +4835,7 @@
       <c r="J68" s="64"/>
       <c r="K68" s="66"/>
     </row>
-    <row r="69" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="69" spans="1:11" s="12" customFormat="1">
       <c r="A69" s="13" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4918,7 +4866,7 @@
       <c r="J69" s="64"/>
       <c r="K69" s="66"/>
     </row>
-    <row r="70" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="70" spans="1:11" s="12" customFormat="1">
       <c r="A70" s="13" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4949,7 +4897,7 @@
       <c r="J70" s="64"/>
       <c r="K70" s="66"/>
     </row>
-    <row r="71" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="71" spans="1:11" s="12" customFormat="1">
       <c r="A71" s="13" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4980,7 +4928,7 @@
       <c r="J71" s="64"/>
       <c r="K71" s="66"/>
     </row>
-    <row r="72" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="72" spans="1:11" s="12" customFormat="1">
       <c r="A72" s="13" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -5011,7 +4959,7 @@
       <c r="J72" s="64"/>
       <c r="K72" s="66"/>
     </row>
-    <row r="73" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="73" spans="1:11" s="12" customFormat="1">
       <c r="A73" s="13" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -5042,7 +4990,7 @@
       <c r="J73" s="64"/>
       <c r="K73" s="66"/>
     </row>
-    <row r="74" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="74" spans="1:11" s="12" customFormat="1">
       <c r="A74" s="13" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -5073,7 +5021,7 @@
       <c r="J74" s="64"/>
       <c r="K74" s="66"/>
     </row>
-    <row r="75" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="75" spans="1:11" s="12" customFormat="1">
       <c r="A75" s="13" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -5104,7 +5052,7 @@
       <c r="J75" s="64"/>
       <c r="K75" s="66"/>
     </row>
-    <row r="76" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="76" spans="1:11" s="12" customFormat="1">
       <c r="A76" s="13" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -5135,7 +5083,7 @@
       <c r="J76" s="64"/>
       <c r="K76" s="66"/>
     </row>
-    <row r="77" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="77" spans="1:11" s="12" customFormat="1">
       <c r="A77" s="13" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -5166,7 +5114,7 @@
       <c r="J77" s="64"/>
       <c r="K77" s="66"/>
     </row>
-    <row r="78" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="78" spans="1:11" s="12" customFormat="1">
       <c r="A78" s="13" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -5197,7 +5145,7 @@
       <c r="J78" s="64"/>
       <c r="K78" s="66"/>
     </row>
-    <row r="79" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="79" spans="1:11" s="12" customFormat="1">
       <c r="A79" s="13" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -5228,7 +5176,7 @@
       <c r="J79" s="64"/>
       <c r="K79" s="66"/>
     </row>
-    <row r="80" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="80" spans="1:11" s="12" customFormat="1">
       <c r="A80" s="13" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -5259,7 +5207,7 @@
       <c r="J80" s="64"/>
       <c r="K80" s="66"/>
     </row>
-    <row r="81" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="81" spans="1:11" s="12" customFormat="1">
       <c r="A81" s="13" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -5290,7 +5238,7 @@
       <c r="J81" s="64"/>
       <c r="K81" s="66"/>
     </row>
-    <row r="82" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="82" spans="1:11" s="12" customFormat="1">
       <c r="A82" s="13" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -5321,7 +5269,7 @@
       <c r="J82" s="64"/>
       <c r="K82" s="66"/>
     </row>
-    <row r="83" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="83" spans="1:11" s="12" customFormat="1">
       <c r="A83" s="13" t="str">
         <f t="shared" ref="A83:A108" si="12">IF(OR(B83&lt;&gt;"",J83&lt;&gt;""),CONCATENATE(LEFT(A82,3),IF(MID(A82,4,2)+1&lt;10,CONCATENATE("0",MID(A82,4,2)+1),MID(A82,4,2)+1)),"")</f>
         <v/>
@@ -5352,7 +5300,7 @@
       <c r="J83" s="64"/>
       <c r="K83" s="66"/>
     </row>
-    <row r="84" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="84" spans="1:11" s="12" customFormat="1">
       <c r="A84" s="13" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5383,7 +5331,7 @@
       <c r="J84" s="64"/>
       <c r="K84" s="66"/>
     </row>
-    <row r="85" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="85" spans="1:11" s="12" customFormat="1">
       <c r="A85" s="13" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5414,7 +5362,7 @@
       <c r="J85" s="64"/>
       <c r="K85" s="66"/>
     </row>
-    <row r="86" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="86" spans="1:11" s="12" customFormat="1">
       <c r="A86" s="13" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5445,7 +5393,7 @@
       <c r="J86" s="64"/>
       <c r="K86" s="66"/>
     </row>
-    <row r="87" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="87" spans="1:11" s="12" customFormat="1">
       <c r="A87" s="13" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5476,7 +5424,7 @@
       <c r="J87" s="64"/>
       <c r="K87" s="66"/>
     </row>
-    <row r="88" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="88" spans="1:11" s="12" customFormat="1">
       <c r="A88" s="13" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5507,7 +5455,7 @@
       <c r="J88" s="64"/>
       <c r="K88" s="66"/>
     </row>
-    <row r="89" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="89" spans="1:11" s="12" customFormat="1">
       <c r="A89" s="13" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5538,7 +5486,7 @@
       <c r="J89" s="64"/>
       <c r="K89" s="66"/>
     </row>
-    <row r="90" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="90" spans="1:11" s="12" customFormat="1">
       <c r="A90" s="13" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5569,7 +5517,7 @@
       <c r="J90" s="64"/>
       <c r="K90" s="66"/>
     </row>
-    <row r="91" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="91" spans="1:11" s="12" customFormat="1">
       <c r="A91" s="13" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5600,7 +5548,7 @@
       <c r="J91" s="64"/>
       <c r="K91" s="66"/>
     </row>
-    <row r="92" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="92" spans="1:11" s="12" customFormat="1">
       <c r="A92" s="13" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5631,7 +5579,7 @@
       <c r="J92" s="64"/>
       <c r="K92" s="66"/>
     </row>
-    <row r="93" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="93" spans="1:11" s="12" customFormat="1">
       <c r="A93" s="13" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5662,7 +5610,7 @@
       <c r="J93" s="64"/>
       <c r="K93" s="66"/>
     </row>
-    <row r="94" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="94" spans="1:11" s="12" customFormat="1">
       <c r="A94" s="13" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5693,7 +5641,7 @@
       <c r="J94" s="64"/>
       <c r="K94" s="66"/>
     </row>
-    <row r="95" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="95" spans="1:11" s="12" customFormat="1">
       <c r="A95" s="13" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5724,7 +5672,7 @@
       <c r="J95" s="64"/>
       <c r="K95" s="66"/>
     </row>
-    <row r="96" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="96" spans="1:11" s="12" customFormat="1">
       <c r="A96" s="13" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5755,7 +5703,7 @@
       <c r="J96" s="64"/>
       <c r="K96" s="66"/>
     </row>
-    <row r="97" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="97" spans="1:11" s="12" customFormat="1">
       <c r="A97" s="13" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5786,7 +5734,7 @@
       <c r="J97" s="64"/>
       <c r="K97" s="66"/>
     </row>
-    <row r="98" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="98" spans="1:11" s="12" customFormat="1">
       <c r="A98" s="13" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5817,7 +5765,7 @@
       <c r="J98" s="64"/>
       <c r="K98" s="66"/>
     </row>
-    <row r="99" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="99" spans="1:11" s="12" customFormat="1">
       <c r="A99" s="13" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5848,7 +5796,7 @@
       <c r="J99" s="64"/>
       <c r="K99" s="66"/>
     </row>
-    <row r="100" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="100" spans="1:11" s="12" customFormat="1">
       <c r="A100" s="13" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5879,7 +5827,7 @@
       <c r="J100" s="64"/>
       <c r="K100" s="66"/>
     </row>
-    <row r="101" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="101" spans="1:11" s="12" customFormat="1">
       <c r="A101" s="13" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5910,7 +5858,7 @@
       <c r="J101" s="64"/>
       <c r="K101" s="66"/>
     </row>
-    <row r="102" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="102" spans="1:11" s="12" customFormat="1">
       <c r="A102" s="13" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5941,7 +5889,7 @@
       <c r="J102" s="64"/>
       <c r="K102" s="66"/>
     </row>
-    <row r="103" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="103" spans="1:11" s="12" customFormat="1">
       <c r="A103" s="13" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5972,7 +5920,7 @@
       <c r="J103" s="64"/>
       <c r="K103" s="66"/>
     </row>
-    <row r="104" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="104" spans="1:11" s="12" customFormat="1">
       <c r="A104" s="13" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -6003,7 +5951,7 @@
       <c r="J104" s="64"/>
       <c r="K104" s="66"/>
     </row>
-    <row r="105" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="105" spans="1:11" s="12" customFormat="1">
       <c r="A105" s="13" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -6034,7 +5982,7 @@
       <c r="J105" s="64"/>
       <c r="K105" s="66"/>
     </row>
-    <row r="106" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="106" spans="1:11" s="12" customFormat="1">
       <c r="A106" s="13" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -6065,7 +6013,7 @@
       <c r="J106" s="64"/>
       <c r="K106" s="66"/>
     </row>
-    <row r="107" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="107" spans="1:11" s="12" customFormat="1">
       <c r="A107" s="13" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -6167,17 +6115,6 @@
       <formula1>INDIRECT(IF(ISERROR(FIND(" ",$E$9)),$E$9,MID($E$9,1,FIND(" ",$E$9))))</formula1>
     </dataValidation>
   </dataValidations>
-  <hyperlinks>
-    <hyperlink ref="B10" r:id="rId1"/>
-    <hyperlink ref="B11" r:id="rId2"/>
-    <hyperlink ref="B12" r:id="rId3"/>
-    <hyperlink ref="B17" r:id="rId4"/>
-    <hyperlink ref="B18" r:id="rId5"/>
-    <hyperlink ref="B19" r:id="rId6"/>
-    <hyperlink ref="B21" r:id="rId7"/>
-    <hyperlink ref="B22" r:id="rId8"/>
-    <hyperlink ref="B26" r:id="rId9"/>
-  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
@@ -6191,10 +6128,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Hoja2" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:L45"/>
+  <dimension ref="A1:K45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6208,7 +6145,7 @@
     <col min="12" max="16384" width="10.83203125" style="23"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="16.25" thickBot="1">
+    <row r="1" spans="1:11" ht="16" thickBot="1">
       <c r="A1" s="90" t="s">
         <v>38</v>
       </c>
@@ -6218,7 +6155,7 @@
       <c r="E1" s="91"/>
       <c r="F1" s="92"/>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:11">
       <c r="A2" s="31" t="s">
         <v>42</v>
       </c>
@@ -6230,7 +6167,7 @@
       <c r="E2" s="95"/>
       <c r="F2" s="33"/>
     </row>
-    <row r="3" spans="1:12" ht="63.25">
+    <row r="3" spans="1:11" ht="60">
       <c r="A3" s="34" t="s">
         <v>43</v>
       </c>
@@ -6254,7 +6191,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="31.75">
+    <row r="4" spans="1:11" ht="30">
       <c r="A4" s="31" t="s">
         <v>44</v>
       </c>
@@ -6282,7 +6219,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="76" thickBot="1">
+    <row r="5" spans="1:11" ht="76" thickBot="1">
       <c r="A5" s="34" t="s">
         <v>45</v>
       </c>
@@ -6292,7 +6229,7 @@
       </c>
       <c r="D5" s="102" t="str">
         <f>CONCATENATE(H21,"_",I21,"_",J21,"_CO")</f>
-        <v>CN_10_03_CO</v>
+        <v>LE_07_04_CO</v>
       </c>
       <c r="E5" s="103"/>
       <c r="F5" s="33"/>
@@ -6308,11 +6245,8 @@
       <c r="K5" s="23">
         <v>2</v>
       </c>
-      <c r="L5" s="23" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="32" thickBot="1">
+    </row>
+    <row r="6" spans="1:11" ht="31" thickBot="1">
       <c r="A6" s="31" t="s">
         <v>10</v>
       </c>
@@ -6334,7 +6268,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="32" thickBot="1">
+    <row r="7" spans="1:11" ht="46" thickBot="1">
       <c r="A7" s="34" t="s">
         <v>11</v>
       </c>
@@ -6344,7 +6278,7 @@
       </c>
       <c r="D7" s="88" t="str">
         <f>CONCATENATE("SolicitudGrafica_",D5,".xls")</f>
-        <v>SolicitudGrafica_CN_10_03_CO.xls</v>
+        <v>SolicitudGrafica_LE_07_04_CO.xls</v>
       </c>
       <c r="E7" s="88"/>
       <c r="F7" s="89"/>
@@ -6361,7 +6295,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="47.5">
+    <row r="8" spans="1:11" ht="45">
       <c r="A8" s="34" t="s">
         <v>53</v>
       </c>
@@ -6380,7 +6314,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="47.5">
+    <row r="9" spans="1:11" ht="45">
       <c r="A9" s="34" t="s">
         <v>12</v>
       </c>
@@ -6399,7 +6333,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="32" thickBot="1">
+    <row r="10" spans="1:11" ht="31" thickBot="1">
       <c r="A10" s="35" t="s">
         <v>36</v>
       </c>
@@ -6418,7 +6352,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:11">
       <c r="I11" s="23" t="s">
         <v>32</v>
       </c>
@@ -6429,7 +6363,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="16.25" thickBot="1">
+    <row r="12" spans="1:11" ht="16" thickBot="1">
       <c r="I12" s="23" t="s">
         <v>37</v>
       </c>
@@ -6440,7 +6374,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:11">
       <c r="A13" s="90" t="s">
         <v>41</v>
       </c>
@@ -6459,7 +6393,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="16.25" thickBot="1">
+    <row r="14" spans="1:11" ht="16" thickBot="1">
       <c r="A14" s="34"/>
       <c r="B14" s="32"/>
       <c r="C14" s="32"/>
@@ -6476,7 +6410,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:11">
       <c r="A15" s="31" t="s">
         <v>46</v>
       </c>
@@ -6494,7 +6428,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="67" customHeight="1">
+    <row r="16" spans="1:11" ht="67" customHeight="1">
       <c r="A16" s="34" t="s">
         <v>47</v>
       </c>
@@ -6528,7 +6462,7 @@
       </c>
       <c r="D17" s="96" t="str">
         <f>CONCATENATE(H21,"_",I21,"_",J21,"_",K45)</f>
-        <v>CN_10_03_REC10</v>
+        <v>LE_07_04_REC10</v>
       </c>
       <c r="E17" s="97"/>
       <c r="F17" s="98"/>
@@ -6539,7 +6473,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="79.5" thickBot="1">
+    <row r="18" spans="1:11" ht="76" thickBot="1">
       <c r="A18" s="34" t="s">
         <v>48</v>
       </c>
@@ -6549,7 +6483,7 @@
       </c>
       <c r="D18" s="88" t="str">
         <f>CONCATENATE("SolicitudGrafica_",D17,".xls")</f>
-        <v>SolicitudGrafica_CN_10_03_REC10.xls</v>
+        <v>SolicitudGrafica_LE_07_04_REC10.xls</v>
       </c>
       <c r="E18" s="88"/>
       <c r="F18" s="89"/>
@@ -6579,7 +6513,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="63.75" thickBot="1">
+    <row r="20" spans="1:11" ht="61" thickBot="1">
       <c r="A20" s="35" t="s">
         <v>51</v>
       </c>
@@ -6589,13 +6523,13 @@
       <c r="E20" s="36"/>
       <c r="F20" s="37"/>
       <c r="H20" s="23">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I20" s="23">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="J20" s="23">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K20" s="23">
         <v>17</v>
@@ -6604,15 +6538,15 @@
     <row r="21" spans="1:11">
       <c r="H21" s="23" t="str">
         <f>IF(INDEX(H4:H7,H20)=H4,"MA",IF(INDEX(H4:H7,H20)=H5,"CN",IF(INDEX(H4:H7,H20)=H6,"CS",IF(INDEX(H4:H7,H20)=H7,"LE"))))</f>
-        <v>CN</v>
+        <v>LE</v>
       </c>
       <c r="I21" s="23" t="str">
         <f>CONCATENATE(IF((I20+2)&lt;10,"0",""),I20+2)</f>
-        <v>10</v>
+        <v>07</v>
       </c>
       <c r="J21" s="23" t="str">
         <f>CONCATENATE(IF(J20&lt;10,"0",""),J20)</f>
-        <v>03</v>
+        <v>04</v>
       </c>
       <c r="K21" s="23">
         <v>18</v>
@@ -6816,10 +6750,10 @@
                     <xdr:rowOff>482600</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
-                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>838200</xdr:colOff>
                     <xdr:row>15</xdr:row>
-                    <xdr:rowOff>723900</xdr:rowOff>
+                    <xdr:rowOff>711200</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -6839,10 +6773,10 @@
                     <xdr:rowOff>482600</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>6</xdr:col>
-                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:col>5</xdr:col>
+                    <xdr:colOff>838200</xdr:colOff>
                     <xdr:row>15</xdr:row>
-                    <xdr:rowOff>723900</xdr:rowOff>
+                    <xdr:rowOff>711200</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -6879,14 +6813,14 @@
               <controlPr defaultSize="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
-                    <xdr:col>3</xdr:col>
-                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>1054100</xdr:colOff>
                     <xdr:row>4</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>4</xdr:col>
-                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>863600</xdr:colOff>
                     <xdr:row>4</xdr:row>
                     <xdr:rowOff>228600</xdr:rowOff>
                   </to>
@@ -7944,7 +7878,7 @@
       <c r="E43" s="56"/>
       <c r="F43" s="56"/>
     </row>
-    <row r="44" spans="1:9" ht="31.75">
+    <row r="44" spans="1:9" ht="30">
       <c r="A44" s="55" t="s">
         <v>111</v>
       </c>
@@ -7972,7 +7906,7 @@
       <c r="E45" s="56"/>
       <c r="F45" s="56"/>
     </row>
-    <row r="46" spans="1:9" ht="47.5">
+    <row r="46" spans="1:9" ht="45">
       <c r="A46" s="55" t="s">
         <v>165</v>
       </c>

</xml_diff>